<commit_message>
all models and metrics now work with experiments module
</commit_message>
<xml_diff>
--- a/UI/tables/pbc.xlsx
+++ b/UI/tables/pbc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BY11"/>
+  <dimension ref="A1:BY12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4203,6 +4203,93 @@
       <c r="BX11" t="inlineStr"/>
       <c r="BY11" t="inlineStr"/>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CRAID</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="n">
+        <v>0.6348407912831906</v>
+      </c>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="n">
+        <v>0.1432293738820869</v>
+      </c>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
+      <c r="AR12" t="inlineStr"/>
+      <c r="AS12" t="inlineStr"/>
+      <c r="AT12" t="inlineStr"/>
+      <c r="AU12" t="inlineStr"/>
+      <c r="AV12" t="inlineStr"/>
+      <c r="AW12" t="inlineStr"/>
+      <c r="AX12" t="inlineStr"/>
+      <c r="AY12" t="inlineStr"/>
+      <c r="AZ12" t="inlineStr"/>
+      <c r="BA12" t="inlineStr"/>
+      <c r="BB12" t="inlineStr"/>
+      <c r="BC12" t="inlineStr"/>
+      <c r="BD12" t="inlineStr"/>
+      <c r="BE12" t="inlineStr"/>
+      <c r="BF12" t="inlineStr"/>
+      <c r="BG12" t="inlineStr"/>
+      <c r="BH12" t="inlineStr"/>
+      <c r="BI12" t="inlineStr"/>
+      <c r="BJ12" t="inlineStr"/>
+      <c r="BK12" t="inlineStr"/>
+      <c r="BL12" t="inlineStr"/>
+      <c r="BM12" t="inlineStr"/>
+      <c r="BN12" t="inlineStr"/>
+      <c r="BO12" t="inlineStr"/>
+      <c r="BP12" t="inlineStr"/>
+      <c r="BQ12" t="inlineStr"/>
+      <c r="BR12" t="inlineStr"/>
+      <c r="BS12" t="inlineStr"/>
+      <c r="BT12" t="inlineStr"/>
+      <c r="BU12" t="inlineStr"/>
+      <c r="BV12" t="inlineStr"/>
+      <c r="BW12" t="inlineStr"/>
+      <c r="BX12" t="inlineStr"/>
+      <c r="BY12" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>